<commit_message>
Version Post Reunion critica
</commit_message>
<xml_diff>
--- a/Diffupar/ASDWP/Templates/Objetivos Diffupar.xlsx
+++ b/Diffupar/ASDWP/Templates/Objetivos Diffupar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Desktop\General\OBJETIVOS\2024\objetivos para Tableau\02 febrero\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alusoftbi-my.sharepoint.com/personal/mariano_aluzzo_alusoft_com_ar/Documents/Source/Desarrollo BI/DIFFUPAR SAP/Diffupar/ASDWP/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9533A8E1-6B73-4F35-8C1D-5B02055381F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{9533A8E1-6B73-4F35-8C1D-5B02055381F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E735127-55B5-4CE5-85F4-B18C70F351D6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="599" xr2:uid="{9309EE3F-AF23-410B-8F31-1E6C039726B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="599" xr2:uid="{9309EE3F-AF23-410B-8F31-1E6C039726B0}"/>
   </bookViews>
   <sheets>
     <sheet name="OBJETIVO TOTAL" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>TOTAL DIFF REAL</t>
   </si>
@@ -218,7 +218,13 @@
     <t>B24 MERCADO LIBRE</t>
   </si>
   <si>
-    <t>02</t>
+    <t>B24 ABASTO</t>
+  </si>
+  <si>
+    <t>B24 ALTO AVELLANEDA</t>
+  </si>
+  <si>
+    <t>B24 DOT SHOPPING</t>
   </si>
 </sst>
 </file>
@@ -273,21 +279,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="8"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,12 +315,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -371,7 +370,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -392,13 +391,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares 2" xfId="3" xr:uid="{77FFB914-07BB-41FA-A601-988946975633}"/>
@@ -431,13 +431,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -495,14 +495,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>798945</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>95160</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>38085</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>47700</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>143040</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -560,14 +560,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>50845</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>143220</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -625,8 +625,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -685,8 +685,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -745,8 +745,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -805,8 +805,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -865,8 +865,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -925,8 +925,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -985,8 +985,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1045,8 +1045,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1105,8 +1105,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1165,8 +1165,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1225,8 +1225,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1285,8 +1285,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1345,8 +1345,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1405,8 +1405,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1465,8 +1465,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1525,8 +1525,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1585,8 +1585,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1645,8 +1645,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1705,8 +1705,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1765,8 +1765,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1825,8 +1825,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1885,8 +1885,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1945,8 +1945,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2005,8 +2005,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2065,8 +2065,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2125,8 +2125,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2185,8 +2185,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2245,8 +2245,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2305,8 +2305,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2365,8 +2365,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2425,8 +2425,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2485,8 +2485,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2545,8 +2545,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2605,8 +2605,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2665,8 +2665,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2725,8 +2725,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2785,8 +2785,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2845,8 +2845,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2905,8 +2905,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2965,8 +2965,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3025,8 +3025,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3085,7 +3085,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
@@ -3145,7 +3145,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
@@ -3205,8 +3205,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3265,8 +3265,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>142860</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3325,7 +3325,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
@@ -3385,7 +3385,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>828465</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="47880" cy="360"/>
@@ -3445,8 +3445,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3505,8 +3505,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3565,8 +3565,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3625,8 +3625,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3685,8 +3685,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3745,8 +3745,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3805,8 +3805,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3865,8 +3865,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3925,8 +3925,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -3985,8 +3985,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4045,8 +4045,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4105,8 +4105,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4165,8 +4165,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4225,8 +4225,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4285,8 +4285,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4345,8 +4345,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4405,8 +4405,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4465,8 +4465,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4525,8 +4525,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4585,8 +4585,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4645,8 +4645,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4705,8 +4705,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4765,8 +4765,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4825,8 +4825,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4885,8 +4885,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -4945,8 +4945,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5005,8 +5005,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5065,8 +5065,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5125,8 +5125,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5185,8 +5185,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5245,8 +5245,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5305,8 +5305,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5365,8 +5365,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5425,8 +5425,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5485,8 +5485,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5545,8 +5545,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5605,8 +5605,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5665,8 +5665,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5725,8 +5725,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5785,8 +5785,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5845,8 +5845,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5905,8 +5905,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -5965,8 +5965,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6025,8 +6025,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6085,8 +6085,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6145,8 +6145,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6205,8 +6205,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6265,8 +6265,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6325,8 +6325,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6385,8 +6385,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6445,8 +6445,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6505,8 +6505,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6565,8 +6565,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6625,8 +6625,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6685,8 +6685,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -6745,8 +6745,8 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>418740</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="360" cy="360"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -7328,7 +7328,7 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">4 1 768,'-2'70'0,"0"-25"0,3-1 0,6 52 0,0-58 0,-2-13 0,-1 1 0,2 42 0,-7-54 0,1-1 0,1 0 0,0 0 0,6 24 0,14 4 0,-18-36 0,0-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,0 0 0,-1 0 0,1 10 0,-1 1465 0,1-1449 0,9 44 0,0 2 0,-5 68 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">4 1 768,'-2'73'0,"0"-27"0,3 0 0,6 53 0,0-59 0,-2-14 0,-1 0 0,2 45 0,-7-57 0,1 0 0,1-1 0,0 1 0,6 24 0,14 5 0,-18-38 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,0 1 0,-1-1 0,1 10 0,-1 1519 0,1-1502 0,9 46 0,0 2 0,-5 70 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -10044,24 +10044,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67168DFF-55A4-4D2E-9434-C5605DF998C6}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="2" width="21.36328125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -10071,778 +10071,820 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="7">
-        <v>35847565.382592529</v>
-      </c>
-      <c r="C2" s="3">
+        <v>103161220.2</v>
+      </c>
+      <c r="C2" s="12">
         <v>2024</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>59</v>
+      <c r="D2" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="7">
-        <v>11309511.069265189</v>
-      </c>
-      <c r="C3" s="3">
+        <v>23510360.530000001</v>
+      </c>
+      <c r="C3" s="12">
         <v>2024</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>59</v>
+      <c r="D3" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="7">
-        <v>53923613.182712138</v>
-      </c>
-      <c r="C4" s="3">
+        <v>94118777.420000002</v>
+      </c>
+      <c r="C4" s="12">
         <v>2024</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>59</v>
+      <c r="D4" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="7">
-        <v>6924985.4542294731</v>
-      </c>
-      <c r="C5" s="3">
+        <v>30246967.66</v>
+      </c>
+      <c r="C5" s="12">
         <v>2024</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>59</v>
+      <c r="D5" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="7">
-        <v>30826226.033117548</v>
-      </c>
-      <c r="C6" s="3">
+        <v>89967015.469999999</v>
+      </c>
+      <c r="C6" s="12">
         <v>2024</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>59</v>
+      <c r="D6" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="7">
-        <v>14921958.481784079</v>
-      </c>
-      <c r="C7" s="3">
+        <v>73455059.599999994</v>
+      </c>
+      <c r="C7" s="12">
         <v>2024</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>59</v>
+      <c r="D7" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="7">
-        <v>16110911.929999961</v>
-      </c>
-      <c r="C8" s="3">
+        <v>50729775.689999998</v>
+      </c>
+      <c r="C8" s="12">
         <v>2024</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>59</v>
+      <c r="D8" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="7">
-        <v>34212457.553667322</v>
-      </c>
-      <c r="C9" s="3">
+        <v>68377429.840000004</v>
+      </c>
+      <c r="C9" s="12">
         <v>2024</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>59</v>
+      <c r="D9" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="7">
-        <v>78373078</v>
-      </c>
-      <c r="C10" s="3">
+        <v>806400000</v>
+      </c>
+      <c r="C10" s="12">
         <v>2024</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>59</v>
+      <c r="D10" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="7">
-        <v>17507375</v>
-      </c>
-      <c r="C11" s="3">
+        <v>12524141.130000001</v>
+      </c>
+      <c r="C11" s="12">
         <v>2024</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>59</v>
+      <c r="D11" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="7">
-        <v>24227447.257063571</v>
-      </c>
-      <c r="C12" s="3">
+        <v>111069286.2</v>
+      </c>
+      <c r="C12" s="12">
         <v>2024</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>59</v>
+      <c r="D12" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="7">
-        <v>10302023.975128699</v>
-      </c>
-      <c r="C13" s="3">
+        <v>35627015.329999998</v>
+      </c>
+      <c r="C13" s="12">
         <v>2024</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>59</v>
+      <c r="D13" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="7">
-        <v>10461059.908429768</v>
-      </c>
-      <c r="C14" s="3">
+        <v>53774844.030000001</v>
+      </c>
+      <c r="C14" s="12">
         <v>2024</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>59</v>
+      <c r="D14" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="7">
-        <v>22766762.979370799</v>
-      </c>
-      <c r="C15" s="3">
+        <v>55605216.950000003</v>
+      </c>
+      <c r="C15" s="12">
         <v>2024</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>59</v>
+      <c r="D15" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="7">
-        <v>18387594.945567504</v>
-      </c>
-      <c r="C16" s="3">
+        <v>49488492.159999996</v>
+      </c>
+      <c r="C16" s="12">
         <v>2024</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>59</v>
+      <c r="D16" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="7">
-        <v>21169021.03012817</v>
-      </c>
-      <c r="C17" s="3">
+        <v>93514822.420000002</v>
+      </c>
+      <c r="C17" s="12">
         <v>2024</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>59</v>
+      <c r="D17" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="7">
-        <v>11875616.715683348</v>
-      </c>
-      <c r="C18" s="3">
+        <v>68691986.379999995</v>
+      </c>
+      <c r="C18" s="12">
         <v>2024</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>59</v>
+      <c r="D18" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="7">
         <v>0</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="12">
         <v>2024</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>59</v>
+      <c r="D19" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="7">
-        <v>14787442.58098218</v>
-      </c>
-      <c r="C20" s="3">
+        <v>58505707.340000004</v>
+      </c>
+      <c r="C20" s="12">
         <v>2024</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>59</v>
+      <c r="D20" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="7">
-        <v>15758721.446171556</v>
-      </c>
-      <c r="C21" s="3">
+        <v>38189620.079999998</v>
+      </c>
+      <c r="C21" s="12">
         <v>2024</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>59</v>
+      <c r="D21" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="7">
-        <v>6004654.7245265609</v>
-      </c>
-      <c r="C22" s="3">
+        <v>21091362.550000001</v>
+      </c>
+      <c r="C22" s="12">
         <v>2024</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>59</v>
+      <c r="D22" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="7">
-        <v>25866655</v>
-      </c>
-      <c r="C23" s="3">
+        <v>201600000</v>
+      </c>
+      <c r="C23" s="12">
         <v>2024</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>59</v>
+      <c r="D23" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="7">
-        <v>27398182.949077819</v>
-      </c>
-      <c r="C24" s="3">
+        <v>111800458.5</v>
+      </c>
+      <c r="C24" s="12">
         <v>2024</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>59</v>
+      <c r="D24" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="7">
-        <v>31857294.825119942</v>
-      </c>
-      <c r="C25" s="3">
+        <v>97774627.680000007</v>
+      </c>
+      <c r="C25" s="12">
         <v>2024</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>59</v>
+      <c r="D25" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="7">
-        <v>7520929.7419293998</v>
-      </c>
-      <c r="C26" s="3">
+        <v>21199354.010000002</v>
+      </c>
+      <c r="C26" s="12">
         <v>2024</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>59</v>
+      <c r="D26" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="7">
-        <v>13965270.982683964</v>
-      </c>
-      <c r="C27" s="3">
+        <v>36186970.039999999</v>
+      </c>
+      <c r="C27" s="12">
         <v>2024</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>59</v>
+      <c r="D27" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="7">
-        <v>15912417.099734388</v>
-      </c>
-      <c r="C28" s="3">
+        <v>43362681.780000001</v>
+      </c>
+      <c r="C28" s="12">
         <v>2024</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>59</v>
+      <c r="D28" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="7">
-        <v>28206510.512261376</v>
-      </c>
-      <c r="C29" s="3">
+        <v>108223791.7</v>
+      </c>
+      <c r="C29" s="12">
         <v>2024</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>59</v>
+      <c r="D29" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="7">
-        <v>21303050.446300309</v>
-      </c>
-      <c r="C30" s="3">
+        <v>108373108.09999999</v>
+      </c>
+      <c r="C30" s="12">
         <v>2024</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>59</v>
+      <c r="D30" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="7">
-        <v>56023414.937248215</v>
-      </c>
-      <c r="C31" s="3">
+        <v>90717643.459999993</v>
+      </c>
+      <c r="C31" s="12">
         <v>2024</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>59</v>
+      <c r="D31" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="7">
-        <v>53385347.217620037</v>
-      </c>
-      <c r="C32" s="3">
+        <v>58534560.740000002</v>
+      </c>
+      <c r="C32" s="12">
         <v>2024</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>59</v>
+      <c r="D32" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="7">
-        <v>23752054.942601211</v>
-      </c>
-      <c r="C33" s="3">
+        <v>70001097.340000004</v>
+      </c>
+      <c r="C33" s="12">
         <v>2024</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>59</v>
+      <c r="D33" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="7">
-        <v>14639431.995886264</v>
-      </c>
-      <c r="C34" s="3">
+        <v>11982219.359999999</v>
+      </c>
+      <c r="C34" s="12">
         <v>2024</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>59</v>
+      <c r="D34" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="7">
-        <v>10827545.335501466</v>
-      </c>
-      <c r="C35" s="3">
+        <v>26203351</v>
+      </c>
+      <c r="C35" s="12">
         <v>2024</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>59</v>
+      <c r="D35" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="7">
-        <v>13917960.799261764</v>
-      </c>
-      <c r="C36" s="3">
+        <v>56116262.920000002</v>
+      </c>
+      <c r="C36" s="12">
         <v>2024</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>59</v>
+      <c r="D36" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="7">
-        <v>23575069.754554491</v>
-      </c>
-      <c r="C37" s="3">
+        <v>46504236.380000003</v>
+      </c>
+      <c r="C37" s="12">
         <v>2024</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>59</v>
+      <c r="D37" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="7">
-        <v>20153291.618691638</v>
-      </c>
-      <c r="C38" s="3">
+        <v>90958516.310000002</v>
+      </c>
+      <c r="C38" s="12">
         <v>2024</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>59</v>
+      <c r="D38" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="7">
-        <v>17407067.465696774</v>
-      </c>
-      <c r="C39" s="3">
+        <v>69570483.680000007</v>
+      </c>
+      <c r="C39" s="12">
         <v>2024</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>59</v>
+      <c r="D39" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="7">
-        <v>11716687.302827545</v>
-      </c>
-      <c r="C40" s="3">
+        <v>42371211.420000002</v>
+      </c>
+      <c r="C40" s="12">
         <v>2024</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>59</v>
+      <c r="D40" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="7">
-        <v>41400953.158077016</v>
-      </c>
-      <c r="C41" s="3">
+        <v>93738169.629999995</v>
+      </c>
+      <c r="C41" s="12">
         <v>2024</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>59</v>
+      <c r="D41" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="7">
-        <v>33742114.801402807</v>
-      </c>
-      <c r="C42" s="3">
+        <v>93644219.219999999</v>
+      </c>
+      <c r="C42" s="12">
         <v>2024</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>59</v>
+      <c r="D42" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B43" s="7">
-        <v>16180784.140951773</v>
-      </c>
-      <c r="C43" s="3">
+        <v>43201735.600000001</v>
+      </c>
+      <c r="C43" s="12">
         <v>2024</v>
       </c>
-      <c r="D43" s="12" t="s">
-        <v>59</v>
+      <c r="D43" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="7">
-        <v>17538615.9824</v>
-      </c>
-      <c r="C44" s="3">
+        <v>102555828</v>
+      </c>
+      <c r="C44" s="12">
         <v>2024</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>59</v>
+      <c r="D44" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B45" s="8">
-        <v>10000000</v>
-      </c>
-      <c r="C45" s="3">
+        <v>16324607.59</v>
+      </c>
+      <c r="C45" s="12">
         <v>2024</v>
       </c>
-      <c r="D45" s="12" t="s">
-        <v>59</v>
+      <c r="D45" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B46" s="8">
-        <v>8500000</v>
-      </c>
-      <c r="C46" s="3">
+        <v>12820495.050000001</v>
+      </c>
+      <c r="C46" s="12">
         <v>2024</v>
       </c>
-      <c r="D46" s="12" t="s">
-        <v>59</v>
+      <c r="D46" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="8">
-        <v>3800000</v>
-      </c>
-      <c r="C47" s="3">
+        <v>8719512.4389999993</v>
+      </c>
+      <c r="C47" s="12">
         <v>2024</v>
       </c>
-      <c r="D47" s="12" t="s">
-        <v>59</v>
+      <c r="D47" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B48" s="8">
-        <v>5800000</v>
-      </c>
-      <c r="C48" s="3">
+        <v>23360000</v>
+      </c>
+      <c r="C48" s="12">
         <v>2024</v>
       </c>
-      <c r="D48" s="12" t="s">
-        <v>59</v>
+      <c r="D48" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="10" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="8">
+        <v>100800000</v>
+      </c>
+      <c r="C49" s="12">
+        <v>2024</v>
+      </c>
+      <c r="D49" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="8">
         <v>0</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C50" s="12">
         <v>2024</v>
       </c>
-      <c r="D49" s="12" t="s">
-        <v>59</v>
+      <c r="D50" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="8">
-        <v>3700000</v>
-      </c>
-      <c r="C50" s="3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="8">
+        <v>21120000</v>
+      </c>
+      <c r="C51" s="12">
         <v>2024</v>
       </c>
-      <c r="D50" s="12" t="s">
-        <v>59</v>
+      <c r="D51" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51" s="8">
-        <v>7000000</v>
-      </c>
-      <c r="C51" s="3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="8">
+        <v>151200000</v>
+      </c>
+      <c r="C52" s="12">
         <v>2024</v>
       </c>
-      <c r="D51" s="12" t="s">
-        <v>59</v>
+      <c r="D52" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="8">
-        <v>0</v>
-      </c>
-      <c r="C52" s="3">
-        <v>2024</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="8">
-        <v>14500000</v>
-      </c>
-      <c r="C53" s="3">
+        <v>47200000</v>
+      </c>
+      <c r="C53" s="12">
         <v>2024</v>
       </c>
-      <c r="D53" s="12" t="s">
-        <v>59</v>
+      <c r="D53" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="8">
-        <v>9300000</v>
-      </c>
-      <c r="C54" s="3">
+        <v>18240000</v>
+      </c>
+      <c r="C54" s="12">
         <v>2024</v>
       </c>
-      <c r="D54" s="12" t="s">
-        <v>59</v>
+      <c r="D54" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B55" s="8">
-        <v>6500000</v>
-      </c>
-      <c r="C55" s="3">
+        <v>19180547.27</v>
+      </c>
+      <c r="C55" s="12">
         <v>2024</v>
       </c>
-      <c r="D55" s="12" t="s">
-        <v>59</v>
+      <c r="D55" s="12">
+        <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B56" s="8">
-        <v>9650000</v>
-      </c>
-      <c r="C56" s="3">
+        <v>16960000</v>
+      </c>
+      <c r="C56" s="12">
         <v>2024</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>59</v>
+      </c>
+      <c r="B57" s="8">
+        <v>15440000</v>
+      </c>
+      <c r="C57" s="12">
+        <v>2024</v>
+      </c>
+      <c r="D57" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="8">
+        <v>11000000</v>
+      </c>
+      <c r="C58" s="12">
+        <v>2024</v>
+      </c>
+      <c r="D58" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="8">
+        <v>30569071.18</v>
+      </c>
+      <c r="C59" s="12">
+        <v>2024</v>
+      </c>
+      <c r="D59" s="12">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -10851,7 +10893,7 @@
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -10865,6 +10907,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005FB90041E1A0FF489EA534F37E9FDEBA" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cb2d9a79b0ea7370ae86443bf358b1da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9032e3ca858c7afc4e4122878b4284d3">
     <xsd:element name="properties">
@@ -10978,15 +11029,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F9D5C07-56DB-48EC-896F-5756225BEADE}">
   <ds:schemaRefs>
@@ -11003,6 +11045,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5BB810-CC22-4977-ABB2-AF9BCEDE77CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{682791D8-6E1C-46C2-B9C3-53F24484E841}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11016,12 +11066,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5BB810-CC22-4977-ABB2-AF9BCEDE77CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>